<commit_message>
missed status code of POST API for price drop
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -203,6 +203,34 @@
     <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}</t>
   </si>
   <si>
+    <t>product_id (string, required): The unique identifier of the product.
+user_id (string, required): The unique identifier of the user.</t>
+  </si>
+  <si>
+    <t>Allows logged-in users to set an alert for a price drop on a specific product. The alert is triggered when the product's price falls to or below the desired price.</t>
+  </si>
+  <si>
+    <t>{
+  "product_id": "12345",
+  "user_id": "u789",
+  "desired_price": 28000
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "success": true,
+  "message": "Price drop alert set successfully for product ID 12345 at 28000 tk."
+}
+</t>
+  </si>
+  <si>
+    <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}/alerts/price-drop</t>
+  </si>
+  <si>
+    <t>1) retrieving detailed information about a specific product, including prices, special offers, and shipping details from various shops. This feature is activated when a user clicks on a product image and is redirected to a detailed view of the product.
+2) viewing the price history of a product at a particular shop on different days of the last month</t>
+  </si>
+  <si>
     <t xml:space="preserve">{
   "success": true,
   "product_details": {
@@ -233,7 +261,7 @@
         "afterpay": true,
         "free_shipping": false
       }
-    }
+    },
     // More offers
   ],
   "price_history": [
@@ -254,34 +282,6 @@
     // more shops
 }
 </t>
-  </si>
-  <si>
-    <t>product_id (string, required): The unique identifier of the product.
-user_id (string, required): The unique identifier of the user.</t>
-  </si>
-  <si>
-    <t>Allows logged-in users to set an alert for a price drop on a specific product. The alert is triggered when the product's price falls to or below the desired price.</t>
-  </si>
-  <si>
-    <t>{
-  "product_id": "12345",
-  "user_id": "u789",
-  "desired_price": 28000
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "message": "Price drop alert set successfully for product ID 12345 at 28000 tk."
-}
-</t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}/alerts/price-drop</t>
-  </si>
-  <si>
-    <t>1) retrieving detailed information about a specific product, including prices, special offers, and shipping details from various shops. This feature is activated when a user clicks on a product image and is redirected to a detailed view of the product.
-2) viewing the price history of a product at a particular shop on different days of the last month</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -800,33 +800,36 @@
         <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F7" s="1">
         <v>200</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
+      <c r="F8" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ENH] added two more APIs
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>METHOD</t>
   </si>
@@ -283,12 +284,82 @@
 }
 </t>
   </si>
+  <si>
+    <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}/{website_id}/wishlist/add</t>
+  </si>
+  <si>
+    <t>For users to bookmark a product and a specific shop selling that product, as a result, adding it to their wishlist.</t>
+  </si>
+  <si>
+    <t>{
+  "user_id": "u789",
+  "product_id": "12345",
+  "shop_id": "s456",
+  "product_price_estimate": 29999,
+  "status": "pending"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "success": true,
+  "message": "Product added to wishlist successfully."
+}
+</t>
+  </si>
+  <si>
+    <t>user_id (string, required): The unique identifier of the logged-in user.
+product_id (string, required): The unique identifier of the product.
+shop_id (string, required): The unique identifier of the shop.
+product_price_estimate (float, required): The estimated price of the product at the time of bookmarking.
+status (string, required): The status of the product in the wishlist (options: "pending", "bought", "rejected").</t>
+  </si>
+  <si>
+    <t>user dashboard - "Recommended products", "Top offers" and "Trending products" sections.</t>
+  </si>
+  <si>
+    <t>/api/1.0/user/{user_id}/get_products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "success": true,
+  "recommended_products": [
+    {
+      "product_name": "Smartphone XYZ",
+      "image_path": "https://www.techshoppers.com/images/smartphone-xyz.jpg",
+      "short_description": "Latest XYZ smartphone with advanced features",
+      "price_range": "$280 - $320",
+      "number_of_shops": 5,
+      "coupons": [
+         {
+               "offer_id": 1,
+               "code": "AMAZON200", 
+               "discount_percentage": 20,
+               "start_date": "2023-12-27",
+               "end_date": "2024-01-07",
+               "is_free_shopping": false
+          },
+         {
+               "offer_id": 3,
+               "code": "EBAY69", 
+               "discount_percentage": null,
+               "start_date": "2023-12-27",
+               "end_date": "2024-01-07",
+               "is_free_shopping": true
+          },
+          // More coupons
+       ]
+    },
+    // More products
+  ]
+}
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +386,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -345,6 +422,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -709,7 +789,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="210" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="294" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -829,6 +909,46 @@
         <v>33</v>
       </c>
       <c r="F8" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1">
+        <v>200</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FEAT] added admin table and API endpoints for admins
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>METHOD</t>
   </si>
@@ -38,9 +37,6 @@
   </si>
   <si>
     <t>POST</t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/login</t>
   </si>
   <si>
     <t>{
@@ -58,9 +54,6 @@
   </si>
   <si>
     <t>user wants to register by providing their personal info</t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/register</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -87,13 +80,7 @@
     <t>GET</t>
   </si>
   <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/search</t>
-  </si>
-  <si>
     <t>https://www.TechShoppers.com/api/1.0/products/search?category=electronics&amp;subcategory=computer&amp;query=laptop</t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/reviews</t>
   </si>
   <si>
     <t>To  display user feedback and overall satisfaction levels regarding TechShoppers' services on the homepage</t>
@@ -137,9 +124,6 @@
 Sorting
 sort_by (string, optional): Sort by a specific field (e.g., "price", "rating").
 sort_order (string, optional): Sort order ("asc" for ascending, "desc" for descending).</t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/filter</t>
   </si>
   <si>
     <t>sorting and filtering products based on various properties. This feature allows users to refine their product search results according to specific criteria like brand, price range, customer reviews, and more</t>
@@ -201,9 +185,6 @@
 subcategory - Search for a specific subcategory of a category of a product (allowed values: electronics - computers, cell-phones, headphones, camera)</t>
   </si>
   <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}</t>
-  </si>
-  <si>
     <t>product_id (string, required): The unique identifier of the product.
 user_id (string, required): The unique identifier of the user.</t>
   </si>
@@ -223,9 +204,6 @@
   "message": "Price drop alert set successfully for product ID 12345 at 28000 tk."
 }
 </t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}/alerts/price-drop</t>
   </si>
   <si>
     <t>1) retrieving detailed information about a specific product, including prices, special offers, and shipping details from various shops. This feature is activated when a user clicks on a product image and is redirected to a detailed view of the product.
@@ -285,9 +263,6 @@
 </t>
   </si>
   <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/details/{user_id}/{product_id}/{website_id}/wishlist/add</t>
-  </si>
-  <si>
     <t>For users to bookmark a product and a specific shop selling that product, as a result, adding it to their wishlist.</t>
   </si>
   <si>
@@ -315,9 +290,6 @@
   </si>
   <si>
     <t>user dashboard - "Recommended products", "Top offers" and "Trending products" sections.</t>
-  </si>
-  <si>
-    <t>/api/1.0/user/{user_id}/get_products</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -354,12 +326,286 @@
 }
 </t>
   </si>
+  <si>
+    <t>users can view and update their profile settings. The profile includes information such as name, password, email, contact number, and address. Additionally, the profile page displays the user's registration date, which is not editable by the user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "success": true,
+  "user_profile": {
+    "name": "John Doe",
+    "email": "johndoe@example.com",
+    "contact_no": "+123456789",
+    "address": "1234 Main St, Dhaka, Bangladesh",
+    "registration_date": "2021-01-01"
+  }
+}
+</t>
+  </si>
+  <si>
+    <t>users can update their personal information</t>
+  </si>
+  <si>
+    <t>{
+  "user_id": "u12345",
+  "name": "Jane Doe",
+  "password": "newPassword123",
+  "email": "janedoe@example.com",
+  "contact_no": "+987654321",
+  "address": "4321 Side St, Dhaka, Bangladesh"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "message": "Profile updated successfully."
+}</t>
+  </si>
+  <si>
+    <t>allows users to retrieve information about their notifications, including the title, message, date created, and notification type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "success": true,
+  "notifications": [
+    {
+      "notification_id": "n123",
+      "title": "Price Drop Alert",
+      "message": "The price of your bookmarked smartphone has dropped!",
+      "date_created": "2023-01-15",
+      "is_read": false,
+      "notification_type": "Price Drop"
+    },
+    {
+      "notification_id": "n124",
+      "title": "New Product Launch",
+      "message": "Explore our latest collection of smartwatches.",
+      "date_created": "2023-02-01",
+      "is_read": true,
+      "notification_type": "New Product"
+    },
+    // More notifications
+  ]
+}
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Base URL: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>https://www.techshoppers.com/1.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>/products/search</t>
+  </si>
+  <si>
+    <t>/reviews</t>
+  </si>
+  <si>
+    <t>/products/filter</t>
+  </si>
+  <si>
+    <t>/products/details/{user_id}/{product_id}</t>
+  </si>
+  <si>
+    <t>/products/details/{user_id}/{product_id}/alerts/price-drop</t>
+  </si>
+  <si>
+    <t>/products/details/{user_id}/{product_id}/{website_id}/wishlist/add</t>
+  </si>
+  <si>
+    <t>/user/{user_id}/get_products</t>
+  </si>
+  <si>
+    <t>/user/{user_id}/viewprofile</t>
+  </si>
+  <si>
+    <t>/user/{user_id}/updateprofile</t>
+  </si>
+  <si>
+    <t>/users/{user_id}/notifications</t>
+  </si>
+  <si>
+    <t>/admin/{admin_id}/websites</t>
+  </si>
+  <si>
+    <t>/admin/{admin_id}/websites/{website_id}/vouchers</t>
+  </si>
+  <si>
+    <t>/admin/{admin_id}/websites/{website_id}/events</t>
+  </si>
+  <si>
+    <t>Get list of all websites currently affiliated with TechShoppers</t>
+  </si>
+  <si>
+    <t>Get all events that a website has invited the admin to</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "websites": [
+    {
+      "website_id": "w123",
+      "website_name": "ebay",
+      "website_url": "https://www.ebay.com"
+    },
+    // More websites
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Get all vouchers offerred by a website to the users</t>
+  </si>
+  <si>
+    <t>/admin/{admin_id}/websites/{website_id}/coupons</t>
+  </si>
+  <si>
+    <t>Get all the coupons offerred by a website on some products</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "coupons": [
+    {
+      "voucher_id": "o123",
+      "user_id": "u123",
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "Get 50% off your next purchase"
+    },
+    {
+      "voucher_id": "o123",
+      "user_id": "u124",
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "Flash sale - for 24 hours only"
+    },
+    // More vouchers
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "coupons": [
+    {
+      "coupon_id": "o123",
+      "code" : EBAY123,
+      "product_id": "p12345",
+      "product_name": "ASUS X122 Gaming Laptop",
+      "price": 80000,
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "10% off"
+    },
+    {
+      "coupon_id": "o123",
+      "code" : AMAZON123,
+      "product_id": "p12346",
+      "product_name": "Oraimo Brass Earphones",
+      "price": 250,
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "Buy one, get one free"
+    },
+    // More coupons
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "events": [
+    {
+      "event_id": "evt123",
+      "name": "Summer Gadget Expo",
+      "venue": "Tech Convention Center, Techville",
+      "description": "An expo showcasing the latest in summer gadgets",
+      "start_date": 2024-01-15,
+      "end_date": 2024-01-21,
+      "activities": [
+           {
+                "date": 2024-01-15,
+                "title": Product Launches,
+                "start_time": "6:00 pm",
+                "end_time": "7:00 pm",
+                "description": "Lorem ipsum dolor sit amet, consectetur adipiscing elit",
+                "venue": "Bayshore Room"
+           },
+           // More activities
+       ]
+    },
+    // More events
+  ]
+}</t>
+  </si>
+  <si>
+    <t>/admin/{admin_id}/websites/events/advertise</t>
+  </si>
+  <si>
+    <t>This endpoint is used by the admin to advertise an event to users and organize a lottery to select winners.</t>
+  </si>
+  <si>
+    <t>{
+  "website_id" : "w123",
+  "event_id": "evt123",
+  "advertise_to_users": true,
+  "lottery_details": {
+    "number_of_winners": 5
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "message": "Event advertised to users and lottery initiated."
+}</t>
+  </si>
+  <si>
+    <t>/admin/{admin_id}/websites/events/notify</t>
+  </si>
+  <si>
+    <t>This endpoint allows the admin to notify selected lottery winners and send them vouchers for the event.</t>
+  </si>
+  <si>
+    <t>{
+  "event_id": "evt123",
+  "winners": ["user123", "user456", "user789", "user101", "user202"]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "success": true,
+  "message": "Winners notified and vouchers sent."
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +635,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -728,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -746,209 +999,377 @@
     <col min="8" max="16384" width="20.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="126" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="294" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="294" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F4" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1">
+        <v>200</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="315" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="1">
-        <v>200</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="315" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" s="1">
         <v>200</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1">
+        <v>200</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="1">
-        <v>200</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="126" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F8" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="126" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1">
+        <v>200</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="198" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="F12" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="252" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="1">
-        <v>200</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F13" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="F14" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="405.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="312" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="390" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="1">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[DOCS] adjusted the fonts and cell size a bit
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[DOCS] Changed structure of response body of the API endpoint for product search
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>METHOD</t>
   </si>
@@ -80,13 +81,7 @@
     <t>GET</t>
   </si>
   <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/search?category=electronics&amp;subcategory=computer&amp;query=laptop</t>
-  </si>
-  <si>
     <t>To  display user feedback and overall satisfaction levels regarding TechShoppers' services on the homepage</t>
-  </si>
-  <si>
-    <t>user selects a category, e.g. "electronics", subcategory, e.g. "Computer" and then types the name of the product , e.g. "laptop"</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -178,11 +173,6 @@
         ]
     }
 }</t>
-  </si>
-  <si>
-    <t>query - The search term e.g. "laptop".
-category - Search for a specific category of product (allowed values: electronics, books, fashion, sports, arts &amp; crafts)
-subcategory - Search for a specific subcategory of a category of a product (allowed values: electronics - computers, cell-phones, headphones, camera)</t>
   </si>
   <si>
     <t>product_id (string, required): The unique identifier of the product.
@@ -598,6 +588,197 @@
     <t>{
   "success": true,
   "message": "Winners notified and vouchers sent."
+}</t>
+  </si>
+  <si>
+    <t>user selects a category, e.g. "computers", subcategory, e.g. "laptop" or just types the name of the product , e.g. "laptop", "asus" etc.</t>
+  </si>
+  <si>
+    <t>https://www.TechShoppers.com/api/1.0/products/search?category=computers&amp;subcategory=laptop&amp;query=asus</t>
+  </si>
+  <si>
+    <t>query - The search term e.g. "asus".
+category - Search for a specific category of product (allowed values: computers, books, fashion, sports, arts &amp; crafts)
+subcategory - Search for a specific subcategory of a category of a product (allowed values: computers - laptop, desktop, pc)</t>
+  </si>
+  <si>
+    <t>{
+    "products": {
+        "items": [
+            {
+                "category": "computers",
+                "subcategory": "laptop",
+                "brands": [
+                {
+                    "brand_name" : "HP",
+                    "available_count": 15,
+                    "platform_products": [
+                    {
+                        "website_name": "amazon",
+                        "website_url": "https://www.amazon.com",
+                        "products_info": [
+                        {
+                            "product_id": "2457",
+                            "product_name": "HP 14 Laptop, Intel Celeron N4020",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/81vzIB8T1wS._AC_SL1500_.jpg",
+                            "price": 60000,
+                            "specs": {
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Celeron Processor N4020",
+                                  "ProcessorFrequency": "1.10 GHz up to 2.80 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 2,
+                                  "CPUCache": "4MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": 14,
+                                  "DisplayType": "LED",
+                                  "DisplayResolution": "HD (1366X768)",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "4GB(onboard)",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "2666MHz"
+                                }
+                            },
+                            "coupon" : {
+                                "code":"SAVE15LAPTOP",
+                                "discount_percentage": 15,
+                                "discount_amount": null,
+                                "description":"Save 15% on selected laptop brands",
+                                "terms":"Valid on specific brands only. Excludes already discounted items",
+                                "start_date":"2024-01-08",
+                                "end_date":"2024-01-10"
+                            },
+                            "rating": 4.5
+                        },
+                        {
+                            "product_id": "2458",
+                            "product_name": "Hp 15.6\" HD Laptop Intel N200 (Pentium) Processor",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/51KupiNLuHL._AC_SL1280_.jpg",
+                            "price": 30000,
+                            "specs":{
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Core i3-1115G4",
+                                  "ProcessorFrequency": "3.00 GHz up to 4.10 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 4,
+                                  "CPUCache": "6 MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": "15.6 Inch",
+                                  "DisplayType": "FHD LED",
+                                  "DisplayResolution": "1920 x 1080",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "8GB",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "3200MHz"
+                                }
+                            },                              
+                            "coupon" : {
+                                "code":"CASHBACK64",
+                                "discount_percentage": null,
+                                "discount_amount": null,
+                                "description":"Receive BDT 6400 cashback on laptops over BDT 28000.",
+                                "terms":"Cashback to be credited after purchase. Applies only to full-priced laptops.",
+                                "start_date":"2024-01-09",
+                                "end_date":"2024-01-11"
+                            },
+                            "rating": 4.4
+                        }
+                        ]
+                    },
+                    {
+                        "website_name": "ebay",
+                        "website_url": "https://www.ebay.com",
+                        "products_info": [
+                        {
+                            "product_id": "2457",
+                            "product_name": "HP 14 Laptop, Intel Celeron N4020",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/81vzIB8T1wS._AC_SL1500_.jpg",
+                            "price": 65000,
+                            "specs": {
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Celeron Processor N4020",
+                                  "ProcessorFrequency": "1.10 GHz up to 2.80 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 2,
+                                  "CPUCache": "4MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": 14,
+                                  "DisplayType": "LED",
+                                  "DisplayResolution": "HD (1366X768)",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "4GB(onboard)",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "2666MHz"
+                                }
+                            },
+                            "coupon" : {
+                                "code":"SAVE12LAPTOP",
+                                "discount_percentage": 12,
+                                "discount_amount": null,
+                                "description":"Save 12% on selected laptop brands",
+                                "terms":"Valid on specific brands only. Excludes already discounted items",
+                                "start_date":"2024-01-06",
+                                "end_date":"2024-01-10"
+                            },
+                            "rating": 4.3
+                        },
+                        {
+                            "product_id": "2458",
+                            "product_name": "Hp 15.6\" HD Laptop Intel N200 (Pentium) Processor",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/51KupiNLuHL._AC_SL1280_.jpg",
+                            "price": 38000,
+                            "specs":{
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Core i3-1115G4",
+                                  "ProcessorFrequency": "3.00 GHz up to 4.10 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 4,
+                                  "CPUCache": "6 MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": "15.6 Inch",
+                                  "DisplayType": "FHD LED",
+                                  "DisplayResolution": "1920 x 1080",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "8GB",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "3200MHz"
+                                }
+                            },
+                            "coupon" : {
+                                "code":"CASHBACK63",
+                                "discount_percentage": null,
+                                "discount_amount": null,
+                                "description":"Receive BDT 6300 cashback on laptops over BDT 28000.",
+                                "terms":"Cashback to be credited after purchase. Applies only to full-priced laptops.",
+                                "start_date":"2024-01-07",
+                                "end_date":"2024-01-09"
+                            },
+                            "rating": 4.1
+                        }
+                        ]
+                    }
+                    ]
+                }, // more brands
+                ]
+            }
+        ]
+    }
 }</t>
   </si>
 </sst>
@@ -983,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -993,7 +1174,7 @@
     <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="84.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="145.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="116" style="1" customWidth="1"/>
     <col min="8" max="16384" width="20.77734375" style="1"/>
@@ -1002,7 +1183,7 @@
     <row r="1" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -1025,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="126" x14ac:dyDescent="0.3">
@@ -1033,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -1053,7 +1234,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -1073,22 +1254,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>74</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="F5" s="1">
         <v>200</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="315" x14ac:dyDescent="0.3">
@@ -1096,13 +1277,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>200</v>
@@ -1113,22 +1294,22 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="1">
         <v>200</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1136,36 +1317,36 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1">
         <v>200</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="126" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1">
         <v>200</v>
@@ -1176,22 +1357,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1">
+        <v>200</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1">
-        <v>200</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1199,13 +1380,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1">
         <v>200</v>
@@ -1216,13 +1397,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1">
         <v>200</v>
@@ -1233,16 +1414,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1">
         <v>200</v>
@@ -1253,13 +1434,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1">
         <v>200</v>
@@ -1270,13 +1451,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F15" s="1">
         <v>200</v>
@@ -1287,13 +1468,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="F16" s="1">
         <v>200</v>
@@ -1304,13 +1485,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F17" s="1">
         <v>200</v>
@@ -1321,13 +1502,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F18" s="1">
         <v>200</v>
@@ -1338,16 +1519,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F19" s="1">
         <v>200</v>
@@ -1358,16 +1539,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="F20" s="1">
         <v>200</v>

</xml_diff>

<commit_message>
[DOCS] Changed the categories and subcategories types in APi Docs
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>METHOD</t>
   </si>
@@ -80,13 +81,7 @@
     <t>GET</t>
   </si>
   <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/search?category=electronics&amp;subcategory=computer&amp;query=laptop</t>
-  </si>
-  <si>
     <t>To  display user feedback and overall satisfaction levels regarding TechShoppers' services on the homepage</t>
-  </si>
-  <si>
-    <t>user selects a category, e.g. "electronics", subcategory, e.g. "Computer" and then types the name of the product , e.g. "laptop"</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -178,11 +173,6 @@
         ]
     }
 }</t>
-  </si>
-  <si>
-    <t>query - The search term e.g. "laptop".
-category - Search for a specific category of product (allowed values: electronics, books, fashion, sports, arts &amp; crafts)
-subcategory - Search for a specific subcategory of a category of a product (allowed values: electronics - computers, cell-phones, headphones, camera)</t>
   </si>
   <si>
     <t>product_id (string, required): The unique identifier of the product.
@@ -598,6 +588,197 @@
     <t>{
   "success": true,
   "message": "Winners notified and vouchers sent."
+}</t>
+  </si>
+  <si>
+    <t>user selects a category, e.g. "computers", subcategory, e.g. "laptop" or just types the name of the product , e.g. "laptop", "asus" etc.</t>
+  </si>
+  <si>
+    <t>https://www.TechShoppers.com/api/1.0/products/search?category=computers&amp;subcategory=laptop&amp;query=asus</t>
+  </si>
+  <si>
+    <t>query - The search term e.g. "asus".
+category - Search for a specific category of product (allowed values: computers, books, fashion, sports, arts &amp; crafts)
+subcategory - Search for a specific subcategory of a category of a product (allowed values: computers - laptop, desktop, pc)</t>
+  </si>
+  <si>
+    <t>{
+    "products": {
+        "items": [
+            {
+                "category": "computers",
+                "subcategory": "laptop",
+                "brands": [
+                {
+                    "brand_name" : "HP",
+                    "available_count": 15,
+                    "platform_products": [
+                    {
+                        "website_name": "amazon",
+                        "website_url": "https://www.amazon.com",
+                        "products_info": [
+                        {
+                            "product_id": "2457",
+                            "product_name": "HP 14 Laptop, Intel Celeron N4020",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/81vzIB8T1wS._AC_SL1500_.jpg",
+                            "price": 60000,
+                            "specs": {
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Celeron Processor N4020",
+                                  "ProcessorFrequency": "1.10 GHz up to 2.80 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 2,
+                                  "CPUCache": "4MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": 14,
+                                  "DisplayType": "LED",
+                                  "DisplayResolution": "HD (1366X768)",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "4GB(onboard)",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "2666MHz"
+                                }
+                            },
+                            "coupon" : {
+                                "code":"SAVE15LAPTOP",
+                                "discount_percentage": 15,
+                                "discount_amount": null,
+                                "description":"Save 15% on selected laptop brands",
+                                "terms":"Valid on specific brands only. Excludes already discounted items",
+                                "start_date":"2024-01-08",
+                                "end_date":"2024-01-10"
+                            },
+                            "rating": 4.5
+                        },
+                        {
+                            "product_id": "2458",
+                            "product_name": "Hp 15.6\" HD Laptop Intel N200 (Pentium) Processor",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/51KupiNLuHL._AC_SL1280_.jpg",
+                            "price": 30000,
+                            "specs":{
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Core i3-1115G4",
+                                  "ProcessorFrequency": "3.00 GHz up to 4.10 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 4,
+                                  "CPUCache": "6 MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": "15.6 Inch",
+                                  "DisplayType": "FHD LED",
+                                  "DisplayResolution": "1920 x 1080",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "8GB",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "3200MHz"
+                                }
+                            },                              
+                            "coupon" : {
+                                "code":"CASHBACK64",
+                                "discount_percentage": null,
+                                "discount_amount": null,
+                                "description":"Receive BDT 6400 cashback on laptops over BDT 28000.",
+                                "terms":"Cashback to be credited after purchase. Applies only to full-priced laptops.",
+                                "start_date":"2024-01-09",
+                                "end_date":"2024-01-11"
+                            },
+                            "rating": 4.4
+                        }
+                        ]
+                    },
+                    {
+                        "website_name": "ebay",
+                        "website_url": "https://www.ebay.com",
+                        "products_info": [
+                        {
+                            "product_id": "2457",
+                            "product_name": "HP 14 Laptop, Intel Celeron N4020",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/81vzIB8T1wS._AC_SL1500_.jpg",
+                            "price": 65000,
+                            "specs": {
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Celeron Processor N4020",
+                                  "ProcessorFrequency": "1.10 GHz up to 2.80 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 2,
+                                  "CPUCache": "4MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": 14,
+                                  "DisplayType": "LED",
+                                  "DisplayResolution": "HD (1366X768)",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "4GB(onboard)",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "2666MHz"
+                                }
+                            },
+                            "coupon" : {
+                                "code":"SAVE12LAPTOP",
+                                "discount_percentage": 12,
+                                "discount_amount": null,
+                                "description":"Save 12% on selected laptop brands",
+                                "terms":"Valid on specific brands only. Excludes already discounted items",
+                                "start_date":"2024-01-06",
+                                "end_date":"2024-01-10"
+                            },
+                            "rating": 4.3
+                        },
+                        {
+                            "product_id": "2458",
+                            "product_name": "Hp 15.6\" HD Laptop Intel N200 (Pentium) Processor",
+                            "image": "https://m.media-amazon.com/images/W/MEDIAX_792452-T2/images/I/51KupiNLuHL._AC_SL1280_.jpg",
+                            "price": 38000,
+                            "specs":{
+                                "Processor": {
+                                  "ProcessorBrand": "Intel",
+                                  "ProcessorModel": "Core i3-1115G4",
+                                  "ProcessorFrequency": "3.00 GHz up to 4.10 GHz",
+                                  "ProcessorCore": 2,
+                                  "ProcessorThread": 4,
+                                  "CPUCache": "6 MB"
+                                },
+                                "Display": {
+                                  "DisplaySize": "15.6 Inch",
+                                  "DisplayType": "FHD LED",
+                                  "DisplayResolution": "1920 x 1080",
+                                  "TouchScreen": "No"
+                                },
+                                "Memory": {
+                                  "RAM": "8GB",
+                                  "RAMType": "DDR4",
+                                  "BusSpeed": "3200MHz"
+                                }
+                            },
+                            "coupon" : {
+                                "code":"CASHBACK63",
+                                "discount_percentage": null,
+                                "discount_amount": null,
+                                "description":"Receive BDT 6300 cashback on laptops over BDT 28000.",
+                                "terms":"Cashback to be credited after purchase. Applies only to full-priced laptops.",
+                                "start_date":"2024-01-07",
+                                "end_date":"2024-01-09"
+                            },
+                            "rating": 4.1
+                        }
+                        ]
+                    }
+                    ]
+                }, // more brands
+                ]
+            }
+        ]
+    }
 }</t>
   </si>
 </sst>
@@ -983,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -993,7 +1174,7 @@
     <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="84.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="145.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="116" style="1" customWidth="1"/>
     <col min="8" max="16384" width="20.77734375" style="1"/>
@@ -1002,7 +1183,7 @@
     <row r="1" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -1025,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="126" x14ac:dyDescent="0.3">
@@ -1033,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -1053,7 +1234,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -1073,22 +1254,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>74</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="F5" s="1">
         <v>200</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="315" x14ac:dyDescent="0.3">
@@ -1096,13 +1277,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>200</v>
@@ -1113,22 +1294,22 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="1">
         <v>200</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1136,36 +1317,36 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1">
         <v>200</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="126" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1">
         <v>200</v>
@@ -1176,22 +1357,22 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1">
+        <v>200</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="1">
-        <v>200</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1199,13 +1380,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1">
         <v>200</v>
@@ -1216,13 +1397,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1">
         <v>200</v>
@@ -1233,16 +1414,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1">
         <v>200</v>
@@ -1253,13 +1434,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1">
         <v>200</v>
@@ -1270,13 +1451,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F15" s="1">
         <v>200</v>
@@ -1287,13 +1468,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="F16" s="1">
         <v>200</v>
@@ -1304,13 +1485,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F17" s="1">
         <v>200</v>
@@ -1321,13 +1502,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F18" s="1">
         <v>200</v>
@@ -1338,16 +1519,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F19" s="1">
         <v>200</v>
@@ -1358,16 +1539,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="F20" s="1">
         <v>200</v>

</xml_diff>

<commit_message>
[DOCS] JWT token for Auth, failure scenarios added
</commit_message>
<xml_diff>
--- a/system-design/TechShoppers-API Docs.xlsx
+++ b/system-design/TechShoppers-API Docs.xlsx
@@ -4,28 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Homepage-guest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Success-scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Failure-scenarios" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
   <si>
     <t>METHOD</t>
   </si>
   <si>
     <t>API ENDPOINT</t>
-  </si>
-  <si>
-    <t>EXAMPLE USAGE</t>
   </si>
   <si>
     <t>REQUEST BODY</t>
@@ -44,14 +40,6 @@
   "name": "John Doe",
   "password": "examplePassword123"
 }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "message": "Login successful",
-  "userID": "123456"
-}
-</t>
   </si>
   <si>
     <t>user wants to register by providing their personal info</t>
@@ -68,13 +56,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "message": "Registration successful"
-}
-</t>
-  </si>
-  <si>
     <t>user/admin wants to login to TechShoppers by providing their username and password</t>
   </si>
   <si>
@@ -82,22 +63,6 @@
   </si>
   <si>
     <t>To  display user feedback and overall satisfaction levels regarding TechShoppers' services on the homepage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "data": [
-    {
-      "review_id": "r123",
-      "user_name": "Alice",
-      "rating": 4.5,
-      "comment": "Great experience! Wide variety of products and excellent customer service.",
-      "date_posted": "2023-12-01"
-    },
-    //more reviews
-  ]
-}
-</t>
   </si>
   <si>
     <t>PARAMETERS</t>
@@ -124,57 +89,6 @@
     <t>sorting and filtering products based on various properties. This feature allows users to refine their product search results according to specific criteria like brand, price range, customer reviews, and more</t>
   </si>
   <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/filter?brand=HP&amp;color=black&amp;price_range=30000-50000&amp;RAM_size=8GB&amp;sort_by=price&amp;sort_order=asc</t>
-  </si>
-  <si>
-    <t>{
-    "success": true,
-    "message": "Showing 50 results for \"laptop\".",
-    "results": {
-        "page": 1,
-        "pages": 39,
-        "shown": 50,
-        "total": 1948,
-        "items": [
-            {
-                "category": "electronics",
-    "subcategory": "computer-laptop",
-    "brands": [
-     {
-      "brand_name" : "HP",
-      "available_count": 15,
-      "product_info": [
-       {
-        "id": "2457",
-        "product_name": "HP 14 Laptop, Intel Celeron N4020",
-        "short_desc": "Lorem ipsum dolor sit amet, consectetur adipiscing elit",
-        "lowest_price": 50000,
-        "highest_discount_percentage": 35,
-        "image": "https://www.example.com/cover.png",
-        "platforms": [
-         {
-          "shop_name": "Amazon",
-          "shop_url": "https://www.amazon.com",
-          "icon": "fab fa-steam",
-          "price": 60000,
-          "discount_percentage": 13,
-          "voucher" : null,
-          "rating": 3.5
-         },
-         // more shops selling this product
-        ],
-       },
-       // more products of brand "HP"
-      ]
-     },
-     // more brands
-    ]
-            }
-        ]
-    }
-}</t>
-  </si>
-  <si>
     <t>product_id (string, required): The unique identifier of the product.
 user_id (string, required): The unique identifier of the user.</t>
   </si>
@@ -189,68 +103,8 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "message": "Price drop alert set successfully for product ID 12345 at 28000 tk."
-}
-</t>
-  </si>
-  <si>
     <t>1) retrieving detailed information about a specific product, including prices, special offers, and shipping details from various shops. This feature is activated when a user clicks on a product image and is redirected to a detailed view of the product.
 2) viewing the price history of a product at a particular shop on different days of the last month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "product_details": {
-    "product_id": "12345",
-    "product_name": "Smartphone XYZ",
-    "category_name": "electronics",
-    "subcategory_name": "computer-laptop",
-    "brand_name": "HP",
-    "image_path": "https://www.techshoppers.com/images/smartphone-xyz.jpg"
-  },
-  "offers": [
-    {
-      "shop_name": "ebay",
-      "price": 30000,
-      "special_offer_details": "10% discount on first purchase",
-      "shipping_details": {
-        "affirm": true,
-        "afterpay": false,
-        "free_shipping": true
-      }
-    },
-    {
-      "shop_name": "amazon",
-      "price": 35000,
-      "special_offer_details": null,
-      "shipping_details": {
-        "affirm": false,
-        "afterpay": true,
-        "free_shipping": false
-      }
-    },
-    // More offers
-  ],
-  "price_history": [
-    {
-      "shop_name": "amazon",
-      "history": [
-         {
-             "date": "2023-11-01",
-             "price": 28000
-         },
-         {
-             "date": "2023-11-05",
-             "price": 33000
-         },
-         // more prices on this shop
-      ]
-    },
-    // more shops
-}
-</t>
   </si>
   <si>
     <t>For users to bookmark a product and a specific shop selling that product, as a result, adding it to their wishlist.</t>
@@ -265,13 +119,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "message": "Product added to wishlist successfully."
-}
-</t>
-  </si>
-  <si>
     <t>user_id (string, required): The unique identifier of the logged-in user.
 product_id (string, required): The unique identifier of the product.
 shop_id (string, required): The unique identifier of the shop.
@@ -282,55 +129,7 @@
     <t>user dashboard - "Recommended products", "Top offers" and "Trending products" sections.</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "recommended_products": [
-    {
-      "product_name": "Smartphone XYZ",
-      "image_path": "https://www.techshoppers.com/images/smartphone-xyz.jpg",
-      "short_description": "Latest XYZ smartphone with advanced features",
-      "price_range": "$280 - $320",
-      "number_of_shops": 5,
-      "coupons": [
-         {
-               "offer_id": 1,
-               "code": "AMAZON200", 
-               "discount_percentage": 20,
-               "start_date": "2023-12-27",
-               "end_date": "2024-01-07",
-               "is_free_shopping": false
-          },
-         {
-               "offer_id": 3,
-               "code": "EBAY69", 
-               "discount_percentage": null,
-               "start_date": "2023-12-27",
-               "end_date": "2024-01-07",
-               "is_free_shopping": true
-          },
-          // More coupons
-       ]
-    },
-    // More products
-  ]
-}
-</t>
-  </si>
-  <si>
     <t>users can view and update their profile settings. The profile includes information such as name, password, email, contact number, and address. Additionally, the profile page displays the user's registration date, which is not editable by the user.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "user_profile": {
-    "name": "John Doe",
-    "email": "johndoe@example.com",
-    "contact_no": "+123456789",
-    "address": "1234 Main St, Dhaka, Bangladesh",
-    "registration_date": "2021-01-01"
-  }
-}
-</t>
   </si>
   <si>
     <t>users can update their personal information</t>
@@ -346,61 +145,9 @@
 }</t>
   </si>
   <si>
-    <t>{
-  "success": true,
-  "message": "Profile updated successfully."
-}</t>
-  </si>
-  <si>
     <t>allows users to retrieve information about their notifications, including the title, message, date created, and notification type</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-  "success": true,
-  "notifications": [
-    {
-      "notification_id": "n123",
-      "title": "Price Drop Alert",
-      "message": "The price of your bookmarked smartphone has dropped!",
-      "date_created": "2023-01-15",
-      "is_read": false,
-      "notification_type": "Price Drop"
-    },
-    {
-      "notification_id": "n124",
-      "title": "New Product Launch",
-      "message": "Explore our latest collection of smartwatches.",
-      "date_created": "2023-02-01",
-      "is_read": true,
-      "notification_type": "New Product"
-    },
-    // More notifications
-  ]
-}
-</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Base URL: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>https://www.techshoppers.com/1.0</t>
-    </r>
-  </si>
-  <si>
     <t>/login</t>
   </si>
   <si>
@@ -416,9 +163,6 @@
     <t>/products/filter</t>
   </si>
   <si>
-    <t>/products/details/{user_id}/{product_id}</t>
-  </si>
-  <si>
     <t>/products/details/{user_id}/{product_id}/alerts/price-drop</t>
   </si>
   <si>
@@ -452,19 +196,6 @@
     <t>Get all events that a website has invited the admin to</t>
   </si>
   <si>
-    <t>{
-  "success": true,
-  "websites": [
-    {
-      "website_id": "w123",
-      "website_name": "ebay",
-      "website_url": "https://www.ebay.com"
-    },
-    // More websites
-  ]
-}</t>
-  </si>
-  <si>
     <t>Get all vouchers offerred by a website to the users</t>
   </si>
   <si>
@@ -472,83 +203,6 @@
   </si>
   <si>
     <t>Get all the coupons offerred by a website on some products</t>
-  </si>
-  <si>
-    <t>{
-  "success": true,
-  "coupons": [
-    {
-      "voucher_id": "o123",
-      "user_id": "u123",
-      "start_date": 2023-01-03,
-      "end_date": 2023-01-08,
-      "description": "Get 50% off your next purchase"
-    },
-    {
-      "voucher_id": "o123",
-      "user_id": "u124",
-      "start_date": 2023-01-03,
-      "end_date": 2023-01-08,
-      "description": "Flash sale - for 24 hours only"
-    },
-    // More vouchers
-  ]
-}</t>
-  </si>
-  <si>
-    <t>{
-  "success": true,
-  "coupons": [
-    {
-      "coupon_id": "o123",
-      "code" : EBAY123,
-      "product_id": "p12345",
-      "product_name": "ASUS X122 Gaming Laptop",
-      "price": 80000,
-      "start_date": 2023-01-03,
-      "end_date": 2023-01-08,
-      "description": "10% off"
-    },
-    {
-      "coupon_id": "o123",
-      "code" : AMAZON123,
-      "product_id": "p12346",
-      "product_name": "Oraimo Brass Earphones",
-      "price": 250,
-      "start_date": 2023-01-03,
-      "end_date": 2023-01-08,
-      "description": "Buy one, get one free"
-    },
-    // More coupons
-  ]
-}</t>
-  </si>
-  <si>
-    <t>{
-  "success": true,
-  "events": [
-    {
-      "event_id": "evt123",
-      "name": "Summer Gadget Expo",
-      "venue": "Tech Convention Center, Techville",
-      "description": "An expo showcasing the latest in summer gadgets",
-      "start_date": 2024-01-15,
-      "end_date": 2024-01-21,
-      "activities": [
-           {
-                "date": 2024-01-15,
-                "title": Product Launches,
-                "start_time": "6:00 pm",
-                "end_time": "7:00 pm",
-                "description": "Lorem ipsum dolor sit amet, consectetur adipiscing elit",
-                "venue": "Bayshore Room"
-           },
-           // More activities
-       ]
-    },
-    // More events
-  ]
-}</t>
   </si>
   <si>
     <t>/admin/{admin_id}/websites/events/advertise</t>
@@ -567,12 +221,6 @@
 }</t>
   </si>
   <si>
-    <t>{
-  "success": true,
-  "message": "Event advertised to users and lottery initiated."
-}</t>
-  </si>
-  <si>
     <t>/admin/{admin_id}/websites/events/notify</t>
   </si>
   <si>
@@ -585,16 +233,7 @@
 }</t>
   </si>
   <si>
-    <t>{
-  "success": true,
-  "message": "Winners notified and vouchers sent."
-}</t>
-  </si>
-  <si>
     <t>user selects a category, e.g. "computers", subcategory, e.g. "laptop" or just types the name of the product , e.g. "laptop", "asus" etc.</t>
-  </si>
-  <si>
-    <t>https://www.TechShoppers.com/api/1.0/products/search?category=computers&amp;subcategory=laptop&amp;query=asus</t>
   </si>
   <si>
     <t>query - The search term e.g. "asus".
@@ -781,12 +420,809 @@
     }
 }</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Base URL:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>https://www.techshoppers.com/api</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "data": [
+    {
+      "review_id": "r123",
+      "user_name": "Alice",
+      "rating": 4.5,
+      "comment": "Great experience! Wide variety of products and excellent customer service.",
+      "date_posted": "2023-12-01"
+    },
+    //more reviews
+  ]
+}
+</t>
+  </si>
+  <si>
+    <t>{
+    "message": "Showing 50 results for \"laptop\".",
+    "results": {
+        "page": 1,
+        "pages": 39,
+        "shown": 50,
+        "total": 1948,
+        "items": [
+            {
+                "category": "electronics",
+    "subcategory": "computer-laptop",
+    "brands": [
+     {
+      "brand_name" : "HP",
+      "available_count": 15,
+      "product_info": [
+       {
+        "id": "2457",
+        "product_name": "HP 14 Laptop, Intel Celeron N4020",
+        "short_desc": "Lorem ipsum dolor sit amet, consectetur adipiscing elit",
+        "lowest_price": 50000,
+        "highest_discount_percentage": 35,
+        "image": "https://www.example.com/cover.png",
+        "platforms": [
+         {
+          "shop_name": "Amazon",
+          "shop_url": "https://www.amazon.com",
+          "icon": "fab fa-steam",
+          "price": 60000,
+          "discount_percentage": 13,
+          "voucher" : null,
+          "rating": 3.5
+         },
+         // more shops selling this product
+        ],
+       },
+       // more products of brand "HP"
+      ]
+     },
+     // more brands
+    ]
+            }
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "product_details": {
+    "product_id": "12345",
+    "product_name": "Smartphone XYZ",
+    "category_name": "electronics",
+    "subcategory_name": "computer-laptop",
+    "brand_name": "HP",
+    "image_path": "https://www.techshoppers.com/images/smartphone-xyz.jpg"
+  },
+  "offers": [
+    {
+      "shop_name": "ebay",
+      "price": 30000,
+      "special_offer_details": "10% discount on first purchase",
+      "shipping_details": {
+        "affirm": true,
+        "afterpay": false,
+        "free_shipping": true
+      }
+    },
+    {
+      "shop_name": "amazon",
+      "price": 35000,
+      "special_offer_details": null,
+      "shipping_details": {
+        "affirm": false,
+        "afterpay": true,
+        "free_shipping": false
+      }
+    },
+    // More offers
+  ],
+  "price_history": [
+    {
+      "shop_name": "amazon",
+      "history": [
+         {
+             "date": "2023-11-01",
+             "price": 28000
+         },
+         {
+             "date": "2023-11-05",
+             "price": 33000
+         },
+         // more prices on this shop
+      ]
+    },
+    // more shops
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "message": "Price drop alert set successfully for product ID 12345 at 28000 tk."
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "message": "Product added to wishlist successfully."
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "recommended_products": [
+    {
+      "product_name": "Smartphone XYZ",
+      "image_path": "https://www.techshoppers.com/images/smartphone-xyz.jpg",
+      "short_description": "Latest XYZ smartphone with advanced features",
+      "price_range": "$280 - $320",
+      "number_of_shops": 5,
+      "coupons": [
+         {
+               "offer_id": 1,
+               "code": "AMAZON200", 
+               "discount_percentage": 20,
+               "start_date": "2023-12-27",
+               "end_date": "2024-01-07",
+               "is_free_shopping": false
+          },
+         {
+               "offer_id": 3,
+               "code": "EBAY69", 
+               "discount_percentage": null,
+               "start_date": "2023-12-27",
+               "end_date": "2024-01-07",
+               "is_free_shopping": true
+          },
+          // More coupons
+       ]
+    },
+    // More products
+  ]
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "user_profile": {
+    "name": "John Doe",
+    "email": "johndoe@example.com",
+    "contact_no": "+123456789",
+    "address": "1234 Main St, Dhaka, Bangladesh",
+    "registration_date": "2021-01-01"
+  }
+}
+</t>
+  </si>
+  <si>
+    <t>{
+  "message": "Profile updated successfully."
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "notifications": [
+    {
+      "notification_id": "n123",
+      "title": "Price Drop Alert",
+      "message": "The price of your bookmarked smartphone has dropped!",
+      "date_created": "2023-01-15",
+      "is_read": false,
+      "notification_type": "Price Drop"
+    },
+    {
+      "notification_id": "n124",
+      "title": "New Product Launch",
+      "message": "Explore our latest collection of smartwatches.",
+      "date_created": "2023-02-01",
+      "is_read": true,
+      "notification_type": "New Product"
+    },
+    // More notifications
+  ]
+}
+</t>
+  </si>
+  <si>
+    <t>{
+  "coupons": [
+    {
+      "coupon_id": "o123",
+      "code" : EBAY123,
+      "product_id": "p12345",
+      "product_name": "ASUS X122 Gaming Laptop",
+      "price": 80000,
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "10% off"
+    },
+    {
+      "coupon_id": "o123",
+      "code" : AMAZON123,
+      "product_id": "p12346",
+      "product_name": "Oraimo Brass Earphones",
+      "price": 250,
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "Buy one, get one free"
+    },
+    // More coupons
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "coupons": [
+    {
+      "voucher_id": "o123",
+      "user_id": "u123",
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "Get 50% off your next purchase"
+    },
+    {
+      "voucher_id": "o123",
+      "user_id": "u124",
+      "start_date": 2023-01-03,
+      "end_date": 2023-01-08,
+      "description": "Flash sale - for 24 hours only"
+    },
+    // More vouchers
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "events": [
+    {
+      "event_id": "evt123",
+      "name": "Summer Gadget Expo",
+      "venue": "Tech Convention Center, Techville",
+      "description": "An expo showcasing the latest in summer gadgets",
+      "start_date": 2024-01-15,
+      "end_date": 2024-01-21,
+      "activities": [
+           {
+                "date": 2024-01-15,
+                "title": Product Launches,
+                "start_time": "6:00 pm",
+                "end_time": "7:00 pm",
+                "description": "Lorem ipsum dolor sit amet, consectetur adipiscing elit",
+                "venue": "Bayshore Room"
+           },
+           // More activities
+       ]
+    },
+    // More events
+  ]
+}</t>
+  </si>
+  <si>
+    <t>{
+  "message": "Event advertised to users and lottery initiated."
+}</t>
+  </si>
+  <si>
+    <t>{
+  "message": "Winners notified and vouchers sent."
+}</t>
+  </si>
+  <si>
+    <t>{
+  "websites": [
+    {
+      "website_id": "w123",
+      "website_name": "ebay",
+      "website_url": "https://www.ebay.com"
+    },
+    // More websites
+  ]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "message": "User registered successfully",
+  "userId": "12345"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "message": "Login successful",
+  "token": "eyJhbGciOiJIUzI1NiIsInR5cCI6IkpXVCJ9"
+}
+</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>{
+  "error": "Invalid username or password"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "error": "User already exists"
+}</t>
+  </si>
+  <si>
+    <t>/products/details/{product_id}</t>
+  </si>
+  <si>
+    <t>{
+  "error": "Invalid request parameters"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "error": "Product not found"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+   "error": "User is not logged in"
+}
+</t>
+  </si>
+  <si>
+    <t>retrieving detailed information and price history about a specific product.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /products/filter?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>brand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=HP&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=black&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>price_range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=30000-50000&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>RAM_size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=8GB&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sort_by</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=price&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sort_order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=asc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /products/search?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>category</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=computers&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>subcategory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=laptop&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>query</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>=asus</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /user/{user_id}/get_products
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Authorization:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Bearer &lt;user_access_token&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">GET </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/user/{user_id}/viewprofile
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Authorization:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Bearer &lt;user_access_token&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+   "error": "User is not an administrator"
+}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /admin/{admin_id}/websites
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Authorization:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Bearer &lt;nonadmin_access_token&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /products/search?category=computers&amp;subcategory=laptop&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>searchkey=hp</t>
+    </r>
+  </si>
+  <si>
+    <t>sorting and filtering products based on various properties.</t>
+  </si>
+  <si>
+    <t>Allows logged-in users to set an alert for a price drop on a specific product.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> /products/filter?brand=HP&amp;color=black&amp;price_range=30000-50000&amp;RAM_size=8GB&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sort_by=priceLowToHigh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>&amp;sort_order=asc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">HTTP Status Codes: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>https://en.wikipedia.org/wiki/List_of_HTTP_status_codes</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,6 +1262,30 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -847,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -859,6 +1319,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1164,16 +1627,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="145.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="116" style="1" customWidth="1"/>
@@ -1183,7 +1644,7 @@
     <row r="1" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.3">
@@ -1194,36 +1655,36 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="126" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1">
         <v>200</v>
@@ -1231,19 +1692,19 @@
     </row>
     <row r="4" spans="1:7" ht="294" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="F4" s="1">
         <v>201</v>
@@ -1251,39 +1712,39 @@
     </row>
     <row r="5" spans="1:7" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1">
         <v>200</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="315" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="273" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="F6" s="1">
         <v>200</v>
@@ -1291,62 +1752,62 @@
     </row>
     <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1">
         <v>200</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1">
         <v>200</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1">
         <v>200</v>
@@ -1354,56 +1815,62 @@
     </row>
     <row r="10" spans="1:7" ht="168" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1">
         <v>200</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="F11" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="198" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="180" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1">
         <v>200</v>
@@ -1411,104 +1878,104 @@
     </row>
     <row r="13" spans="1:7" ht="252" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="396" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F15" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="405.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="390" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="312" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="296.39999999999998" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F17" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="390" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1">
         <v>200</v>
@@ -1516,16 +1983,16 @@
     </row>
     <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>68</v>
@@ -1536,19 +2003,19 @@
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="F20" s="1">
         <v>200</v>
@@ -1562,12 +2029,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.77734375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="1">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="294" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="1">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="147" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="1">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>